<commit_message>
changed data function to include cr-28 data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Thrawn\My Lectures\ME 160\Pittoni\Projects\Project BOX\Python CODES\Final TRANSMISSION\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flash\Desktop\ME 1600\ME 1600\Final Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123310A5-BA3B-44B7-9E81-310B62A43B0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24147A81-1535-4AA8-9C45-C7BCA6B134AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="190" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problem Variables" sheetId="1" r:id="rId1"/>
-    <sheet name="Dynamometer" sheetId="2" r:id="rId2"/>
+    <sheet name="cr-28 var" sheetId="3" r:id="rId2"/>
+    <sheet name="Dynamometer" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="50">
   <si>
     <t>DATA FOR THE CAR PERFORMANCE</t>
   </si>
@@ -165,6 +166,12 @@
   </si>
   <si>
     <t>hA/h</t>
+  </si>
+  <si>
+    <t>DATA FOR THE CAR PERFORMANCE CR-28</t>
+  </si>
+  <si>
+    <t>CR-28</t>
   </si>
 </sst>
 </file>
@@ -707,22 +714,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="A1:E30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="58.9296875" customWidth="1"/>
+    <col min="1" max="1" width="58.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -733,7 +740,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -744,7 +751,7 @@
         <v>4.1710000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -755,7 +762,7 @@
         <v>2.34</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -766,7 +773,7 @@
         <v>1.5209999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -777,7 +784,7 @@
         <v>1.143</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -788,7 +795,7 @@
         <v>0.86699999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -799,8 +806,8 @@
         <v>0.69099999999999995</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -814,7 +821,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>27</v>
       </c>
@@ -828,7 +835,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -842,7 +849,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
@@ -856,7 +863,7 @@
         <v>2.31</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
@@ -870,7 +877,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -884,7 +891,7 @@
         <v>1.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>30</v>
       </c>
@@ -898,7 +905,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -912,7 +919,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
@@ -926,7 +933,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>29</v>
       </c>
@@ -940,7 +947,7 @@
         <v>14729</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>34</v>
       </c>
@@ -954,7 +961,7 @@
         <v>1.2250000000000001</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
@@ -968,7 +975,7 @@
         <v>3.46</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
         <v>31</v>
       </c>
@@ -982,8 +989,8 @@
         <v>1.1200000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="25" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="25" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="5" t="s">
         <v>37</v>
       </c>
@@ -997,7 +1004,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="12" t="s">
         <v>38</v>
       </c>
@@ -1011,7 +1018,7 @@
         <v>1.08</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>39</v>
       </c>
@@ -1025,7 +1032,7 @@
         <v>0.70299999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>40</v>
       </c>
@@ -1039,7 +1046,7 @@
         <v>0.59599999999999997</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -1053,7 +1060,7 @@
         <v>0.57599999999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>42</v>
       </c>
@@ -1074,6 +1081,313 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EF4E6B3-C725-4ABF-87A8-842524EB02A4}">
+  <dimension ref="A1:D26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>4.1710000000000003</v>
+      </c>
+      <c r="C4">
+        <v>4.1710000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2.34</v>
+      </c>
+      <c r="C5">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1.5209999999999999</v>
+      </c>
+      <c r="C6">
+        <v>1.5209999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1.143</v>
+      </c>
+      <c r="C7">
+        <v>1.143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="C8">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="C9">
+        <v>0.69099999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>100</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>1.53</v>
+      </c>
+      <c r="D14">
+        <v>1.53</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>0.2</v>
+      </c>
+      <c r="D15">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D16">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="D17">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18">
+        <v>95</v>
+      </c>
+      <c r="D18">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19">
+        <v>98</v>
+      </c>
+      <c r="D19">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="C20">
+        <v>2134</v>
+      </c>
+      <c r="D20">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="D21">
+        <v>1.2250000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22">
+        <v>3.5</v>
+      </c>
+      <c r="D22">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="D23">
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26">
+        <v>2023</v>
+      </c>
+      <c r="C26">
+        <v>1.81</v>
+      </c>
+      <c r="D26">
+        <v>1.07</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B15"/>
   <sheetViews>
@@ -1081,15 +1395,15 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>25</v>
       </c>
@@ -1097,7 +1411,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="12">
         <v>800</v>
       </c>
@@ -1105,7 +1419,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>1312</v>
       </c>
@@ -1113,7 +1427,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>1800</v>
       </c>
@@ -1121,7 +1435,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>2276</v>
       </c>
@@ -1129,7 +1443,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2800</v>
       </c>
@@ -1137,7 +1451,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>3316</v>
       </c>
@@ -1145,7 +1459,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>3806</v>
       </c>
@@ -1153,7 +1467,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>4300</v>
       </c>
@@ -1161,7 +1475,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>4770</v>
       </c>
@@ -1169,7 +1483,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>5300</v>
       </c>
@@ -1177,7 +1491,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>5800</v>
       </c>
@@ -1185,7 +1499,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3">
         <v>6300</v>
       </c>

</xml_diff>

<commit_message>
added cr dyno data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,17 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28227"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\flash\Documents\GitHub\finalproject-p1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D981C9DE-123B-4905-9A42-2087BA9BB7BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="6100" yWindow="3020" windowWidth="19200" windowHeight="11170" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Problem Variables"/>
-    <sheet r:id="rId2" sheetId="2" name="cr-28 var"/>
-    <sheet r:id="rId3" sheetId="3" name="Dynamometer"/>
+    <sheet name="Problem Variables" sheetId="1" r:id="rId1"/>
+    <sheet name="cr-dyno" sheetId="4" r:id="rId2"/>
+    <sheet name="cr-28 var" sheetId="2" r:id="rId3"/>
+    <sheet name="Dynamometer" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -171,9 +178,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -184,7 +190,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFff0000"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
     </font>
@@ -200,6 +206,11 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -369,116 +380,110 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="31">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="12" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -489,10 +494,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -530,71 +535,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -622,7 +627,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -645,11 +650,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -658,13 +663,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -674,7 +679,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -683,7 +688,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -692,7 +697,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -700,10 +705,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -768,159 +773,138 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" style="15" width="58.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="58.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.54296875" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A1" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="11"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="18" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1"/>
+    <row r="3" spans="1:4" ht="19.5" customHeight="1">
+      <c r="A3" s="14" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="20" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="19.5" customHeight="1">
+      <c r="A4" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="21">
-        <v>4.171</v>
-      </c>
-      <c r="C4" s="21">
-        <v>4.171</v>
-      </c>
-      <c r="D4" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="20" t="s">
+      <c r="B4" s="17">
+        <v>4.1710000000000003</v>
+      </c>
+      <c r="C4" s="17">
+        <v>4.1710000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="18">
         <v>2.34</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="18">
         <v>2.34</v>
       </c>
-      <c r="D5" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="20" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A6" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="22">
-        <v>1.521</v>
-      </c>
-      <c r="C6" s="22">
-        <v>1.521</v>
-      </c>
-      <c r="D6" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="20" t="s">
+      <c r="B6" s="18">
+        <v>1.5209999999999999</v>
+      </c>
+      <c r="C6" s="18">
+        <v>1.5209999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="18">
         <v>1.143</v>
       </c>
-      <c r="C7" s="22">
+      <c r="C7" s="18">
         <v>1.143</v>
       </c>
-      <c r="D7" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="20" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A8" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="22">
-        <v>0.867</v>
-      </c>
-      <c r="C8" s="22">
-        <v>0.867</v>
-      </c>
-      <c r="D8" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="23" t="s">
+      <c r="B8" s="18">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="C8" s="18">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A9" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="24">
-        <v>0.691</v>
-      </c>
-      <c r="C9" s="24">
-        <v>0.691</v>
-      </c>
-      <c r="D9" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
-      <c r="A10" s="11"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
-      <c r="A11" s="18" t="s">
+      <c r="B9" s="20">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="C9" s="20">
+        <v>0.69099999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19.5" customHeight="1"/>
+    <row r="11" spans="1:4" ht="19.5" customHeight="1">
+      <c r="A11" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
-      <c r="A12" s="20" t="s">
+    <row r="12" spans="1:4" ht="19.5" customHeight="1">
+      <c r="A12" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="22">
         <v>100</v>
       </c>
-      <c r="D12" s="26">
+      <c r="D12" s="22">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="20" t="s">
+    <row r="13" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="23" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="6">
@@ -930,67 +914,67 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="20" t="s">
+    <row r="14" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A14" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="18">
         <v>2.31</v>
       </c>
-      <c r="D14" s="22">
+      <c r="D14" s="18">
         <v>2.31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="20" t="s">
+    <row r="15" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A15" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="22">
+      <c r="C15" s="18">
         <v>0.19</v>
       </c>
-      <c r="D15" s="22">
+      <c r="D15" s="18">
         <v>0.19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="20" t="s">
+    <row r="16" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A16" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="22">
-        <v>0.018</v>
-      </c>
-      <c r="D16" s="22">
-        <v>0.018</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="20" t="s">
+      <c r="C16" s="18">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D16" s="18">
+        <v>1.7999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A17" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="22">
+      <c r="C17" s="18">
         <v>0.6</v>
       </c>
-      <c r="D17" s="22">
+      <c r="D17" s="18">
         <v>0.6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="20" t="s">
+    <row r="18" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A18" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="23" t="s">
         <v>28</v>
       </c>
       <c r="C18" s="6">
@@ -1000,11 +984,11 @@
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="20" t="s">
+    <row r="19" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A19" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="23" t="s">
         <v>30</v>
       </c>
       <c r="C19" s="6">
@@ -1014,11 +998,11 @@
         <v>98</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="20" t="s">
+    <row r="20" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A20" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="23" t="s">
         <v>32</v>
       </c>
       <c r="C20" s="6">
@@ -1028,135 +1012,130 @@
         <v>14729</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="20" t="s">
+    <row r="21" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A21" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="22">
-        <v>1.225</v>
-      </c>
-      <c r="D21" s="22">
-        <v>1.225</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="20" t="s">
+      <c r="C21" s="18">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="D21" s="18">
+        <v>1.2250000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A22" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="22">
+      <c r="C22" s="18">
         <v>3.46</v>
       </c>
-      <c r="D22" s="22">
+      <c r="D22" s="18">
         <v>3.46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="15.75">
-      <c r="A23" s="23" t="s">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+      <c r="A23" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="24">
-        <v>1.12</v>
-      </c>
-      <c r="D23" s="24">
-        <v>1.12</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="11"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="18" t="s">
+      <c r="C23" s="20">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="D23" s="20">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" customHeight="1"/>
+    <row r="25" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A25" s="14" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="19" t="s">
+      <c r="C25" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="25" t="s">
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="30" t="s">
+    <row r="26" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A26" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="B26" s="26">
+      <c r="B26" s="22">
         <v>2005</v>
       </c>
-      <c r="C26" s="21">
+      <c r="C26" s="17">
         <v>0.4</v>
       </c>
-      <c r="D26" s="31">
+      <c r="D26" s="27">
         <v>1.08</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="20" t="s">
+    <row r="27" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A27" s="16" t="s">
         <v>46</v>
       </c>
       <c r="B27" s="6">
         <v>1992</v>
       </c>
-      <c r="C27" s="22">
+      <c r="C27" s="18">
         <v>0.33</v>
       </c>
-      <c r="D27" s="32">
-        <v>0.703</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="20" t="s">
+      <c r="D27" s="28">
+        <v>0.70299999999999996</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A28" s="16" t="s">
         <v>47</v>
       </c>
       <c r="B28" s="6">
         <v>2003</v>
       </c>
-      <c r="C28" s="22">
+      <c r="C28" s="18">
         <v>0.38</v>
       </c>
-      <c r="D28" s="32">
-        <v>0.596</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="20" t="s">
+      <c r="D28" s="28">
+        <v>0.59599999999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A29" s="16" t="s">
         <v>48</v>
       </c>
       <c r="B29" s="6">
         <v>2014</v>
       </c>
-      <c r="C29" s="22">
+      <c r="C29" s="18">
         <v>0.26</v>
       </c>
-      <c r="D29" s="32">
-        <v>0.576</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="23" t="s">
+      <c r="D29" s="28">
+        <v>0.57599999999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A30" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B30" s="9">
         <v>2014</v>
       </c>
-      <c r="C30" s="24">
-        <v>0.281</v>
-      </c>
-      <c r="D30" s="33">
+      <c r="C30" s="20">
+        <v>0.28100000000000003</v>
+      </c>
+      <c r="D30" s="29">
         <v>0.622</v>
       </c>
     </row>
@@ -1166,7 +1145,122 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1ACE254F-3A95-447B-BD34-DB1202A0F724}">
+  <dimension ref="A4:B16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="4" spans="1:2">
+      <c r="A4" s="30">
+        <v>6000</v>
+      </c>
+      <c r="B4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="30">
+        <v>6500</v>
+      </c>
+      <c r="B5">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="30">
+        <v>7000</v>
+      </c>
+      <c r="B6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="30">
+        <v>7500</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="30">
+        <v>8000</v>
+      </c>
+      <c r="B8">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="30">
+        <v>8500</v>
+      </c>
+      <c r="B9">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="30">
+        <v>9000</v>
+      </c>
+      <c r="B10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="30">
+        <v>9500</v>
+      </c>
+      <c r="B11">
+        <v>32.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="30">
+        <v>10000</v>
+      </c>
+      <c r="B12">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="30">
+        <v>15000</v>
+      </c>
+      <c r="B13">
+        <v>31.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="30">
+        <v>11000</v>
+      </c>
+      <c r="B14">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="30">
+        <v>115000</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="30"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1174,331 +1268,305 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" style="15" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="16" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.54296875" style="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="11"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="11" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="18.75" customHeight="1"/>
+    <row r="3" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="11" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="13">
-        <v>4.171</v>
-      </c>
-      <c r="C4" s="13">
-        <v>4.171</v>
-      </c>
-      <c r="D4" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="11" t="s">
+      <c r="B4" s="11">
+        <v>4.1710000000000003</v>
+      </c>
+      <c r="C4" s="11">
+        <v>4.1710000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="11">
         <v>2.34</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="11">
         <v>2.34</v>
       </c>
-      <c r="D5" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="11" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="13">
-        <v>1.521</v>
-      </c>
-      <c r="C6" s="13">
-        <v>1.521</v>
-      </c>
-      <c r="D6" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="11" t="s">
+      <c r="B6" s="11">
+        <v>1.5209999999999999</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1.5209999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="11">
         <v>1.143</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="11">
         <v>1.143</v>
       </c>
-      <c r="D7" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="11" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="13">
-        <v>0.867</v>
-      </c>
-      <c r="C8" s="13">
-        <v>0.867</v>
-      </c>
-      <c r="D8" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="11" t="s">
+      <c r="B8" s="11">
+        <v>0.86699999999999999</v>
+      </c>
+      <c r="C8" s="11">
+        <v>0.86699999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="13">
-        <v>0.691</v>
-      </c>
-      <c r="C9" s="13">
-        <v>0.691</v>
-      </c>
-      <c r="D9" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="11"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="11" t="s">
+      <c r="B9" s="11">
+        <v>0.69099999999999995</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0.69099999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18.75" customHeight="1"/>
+    <row r="11" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="11" t="s">
+    <row r="12" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="14">
+      <c r="C12" s="12">
         <v>100</v>
       </c>
-      <c r="D12" s="14">
+      <c r="D12" s="12">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="11" t="s">
+    <row r="13" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="14">
+      <c r="C13" s="12">
         <v>2</v>
       </c>
-      <c r="D13" s="14">
+      <c r="D13" s="12">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A14" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="11">
         <v>1.53</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14" s="11">
         <v>1.53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="11" t="s">
+    <row r="15" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A15" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="11">
         <v>0.2</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15" s="11">
         <v>0.2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="11" t="s">
+    <row r="16" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A16" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="13">
-        <v>0.012</v>
-      </c>
-      <c r="D16" s="13">
-        <v>0.012</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="11" t="s">
+      <c r="C16" s="11">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D16" s="11">
+        <v>1.2E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A17" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="13">
+      <c r="C17" s="11">
         <v>0.5</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17" s="11">
         <v>0.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="11" t="s">
+    <row r="18" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A18" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="14">
+      <c r="C18" s="12">
         <v>95</v>
       </c>
-      <c r="D18" s="14">
+      <c r="D18" s="12">
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="11" t="s">
+    <row r="19" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A19" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="14">
+      <c r="C19" s="12">
         <v>98</v>
       </c>
-      <c r="D19" s="14">
+      <c r="D19" s="12">
         <v>98</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="14">
+      <c r="C20" s="12">
         <v>2134</v>
       </c>
-      <c r="D20" s="14">
+      <c r="D20" s="12">
         <v>2134</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="11" t="s">
+    <row r="21" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A21" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="13">
-        <v>1.225</v>
-      </c>
-      <c r="D21" s="13">
-        <v>1.225</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="11" t="s">
+      <c r="C21" s="11">
+        <v>1.2250000000000001</v>
+      </c>
+      <c r="D21" s="11">
+        <v>1.2250000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A22" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C22" s="13">
+      <c r="C22" s="11">
         <v>3.5</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="11">
         <v>3.5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="11" t="s">
+    <row r="23" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A23" t="s">
         <v>37</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="13">
-        <v>0.765</v>
-      </c>
-      <c r="D23" s="13">
-        <v>0.765</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="11"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="11" t="s">
+      <c r="C23" s="11">
+        <v>0.76500000000000001</v>
+      </c>
+      <c r="D23" s="11">
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="18.75" customHeight="1"/>
+    <row r="25" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A25" t="s">
         <v>39</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="10" t="s">
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="11" t="s">
+    <row r="26" spans="1:4" ht="18.75" customHeight="1">
+      <c r="A26" t="s">
         <v>43</v>
       </c>
-      <c r="B26" s="14">
+      <c r="B26" s="12">
         <v>2023</v>
       </c>
-      <c r="C26" s="13">
+      <c r="C26" s="11">
         <v>1.81</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="11">
         <v>1.07</v>
       </c>
     </row>
@@ -1507,32 +1575,29 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="2" width="13.54296875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="15.75">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="15.75">
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1"/>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1540,7 +1605,7 @@
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1">
       <c r="A4" s="5">
         <v>800</v>
       </c>
@@ -1548,7 +1613,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1">
       <c r="A5" s="7">
         <v>1312</v>
       </c>
@@ -1556,7 +1621,7 @@
         <v>135</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1">
       <c r="A6" s="7">
         <v>1800</v>
       </c>
@@ -1564,7 +1629,7 @@
         <v>148</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1">
       <c r="A7" s="7">
         <v>2276</v>
       </c>
@@ -1572,7 +1637,7 @@
         <v>157</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1">
       <c r="A8" s="7">
         <v>2800</v>
       </c>
@@ -1580,7 +1645,7 @@
         <v>165</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1">
       <c r="A9" s="7">
         <v>3316</v>
       </c>
@@ -1588,7 +1653,7 @@
         <v>172</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1">
       <c r="A10" s="7">
         <v>3806</v>
       </c>
@@ -1596,7 +1661,7 @@
         <v>178</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1">
       <c r="A11" s="7">
         <v>4300</v>
       </c>
@@ -1604,7 +1669,7 @@
         <v>184</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1">
       <c r="A12" s="7">
         <v>4770</v>
       </c>
@@ -1612,7 +1677,7 @@
         <v>188</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1">
       <c r="A13" s="7">
         <v>5300</v>
       </c>
@@ -1620,7 +1685,7 @@
         <v>187</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1">
       <c r="A14" s="7">
         <v>5800</v>
       </c>
@@ -1628,7 +1693,7 @@
         <v>183</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="15.75">
+    <row r="15" spans="1:2" ht="15.75" customHeight="1">
       <c r="A15" s="8">
         <v>6300</v>
       </c>

</xml_diff>